<commit_message>
request excel and send
</commit_message>
<xml_diff>
--- a/DATA SAMPLE/Upload Student bulk xslx.xlsx
+++ b/DATA SAMPLE/Upload Student bulk xslx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\New AMS\DATA SAMPLE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2364E0D-CC2B-4B70-A436-C6CF969B93DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34433D8E-E4D5-49B6-8FFF-C57093C93DE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="4392" windowWidth="17280" windowHeight="8880" xr2:uid="{ADFDEEF2-F542-4A0F-9961-7E34A3842DCC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{ADFDEEF2-F542-4A0F-9961-7E34A3842DCC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="137">
   <si>
     <t>name</t>
   </si>
@@ -66,9 +66,6 @@
     <t>section</t>
   </si>
   <si>
-    <t>batch</t>
-  </si>
-  <si>
     <t>password</t>
   </si>
   <si>
@@ -88,9 +85,6 @@
   </si>
   <si>
     <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
   </si>
   <si>
     <t>medicaps</t>
@@ -879,10 +873,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E5CC03C-5830-4EA6-B66F-4F0087813C23}">
-  <dimension ref="A1:L61"/>
+  <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C61" workbookViewId="0">
-      <selection activeCell="M70" sqref="M70"/>
+    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -896,7 +890,7 @@
     <col min="7" max="7" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -930,16 +924,13 @@
       <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C2">
         <v>2002261</v>
@@ -948,36 +939,33 @@
         <v>7000253811</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H2">
         <v>2020</v>
       </c>
       <c r="I2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>21</v>
-      </c>
       <c r="B3" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C3">
         <v>2002262</v>
@@ -986,36 +974,33 @@
         <v>7000253812</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H3">
         <v>2020</v>
       </c>
       <c r="I3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C4">
         <v>2002263</v>
@@ -1024,36 +1009,33 @@
         <v>7000253813</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H4">
         <v>2020</v>
       </c>
       <c r="I4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K4" t="s">
-        <v>18</v>
-      </c>
-      <c r="L4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C5">
         <v>2002264</v>
@@ -1062,36 +1044,33 @@
         <v>7000253814</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H5">
         <v>2020</v>
       </c>
       <c r="I5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C6">
         <v>2002265</v>
@@ -1100,36 +1079,33 @@
         <v>7000253815</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H6">
         <v>2020</v>
       </c>
       <c r="I6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K6" t="s">
-        <v>18</v>
-      </c>
-      <c r="L6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C7">
         <v>2002266</v>
@@ -1138,36 +1114,33 @@
         <v>7000253816</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H7">
         <v>2020</v>
       </c>
       <c r="I7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K7" t="s">
-        <v>18</v>
-      </c>
-      <c r="L7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C8">
         <v>2002267</v>
@@ -1176,36 +1149,33 @@
         <v>7000253817</v>
       </c>
       <c r="E8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H8">
         <v>2020</v>
       </c>
       <c r="I8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K8" t="s">
-        <v>18</v>
-      </c>
-      <c r="L8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C9">
         <v>2002268</v>
@@ -1214,36 +1184,33 @@
         <v>7000253818</v>
       </c>
       <c r="E9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H9">
         <v>2020</v>
       </c>
       <c r="I9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K9" t="s">
-        <v>18</v>
-      </c>
-      <c r="L9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C10">
         <v>2002269</v>
@@ -1252,36 +1219,33 @@
         <v>7000253819</v>
       </c>
       <c r="E10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H10">
         <v>2020</v>
       </c>
       <c r="I10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K10" t="s">
-        <v>18</v>
-      </c>
-      <c r="L10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C11">
         <v>2002270</v>
@@ -1290,36 +1254,33 @@
         <v>7000253820</v>
       </c>
       <c r="E11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H11">
         <v>2020</v>
       </c>
       <c r="I11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K11" t="s">
-        <v>18</v>
-      </c>
-      <c r="L11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C12">
         <v>2002271</v>
@@ -1328,36 +1289,33 @@
         <v>7000253821</v>
       </c>
       <c r="E12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H12">
         <v>2020</v>
       </c>
       <c r="I12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K12" t="s">
-        <v>18</v>
-      </c>
-      <c r="L12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C13">
         <v>2002272</v>
@@ -1366,36 +1324,33 @@
         <v>7000253822</v>
       </c>
       <c r="E13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H13">
         <v>2020</v>
       </c>
       <c r="I13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K13" t="s">
-        <v>18</v>
-      </c>
-      <c r="L13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C14">
         <v>2002273</v>
@@ -1404,36 +1359,33 @@
         <v>7000253823</v>
       </c>
       <c r="E14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H14">
         <v>2020</v>
       </c>
       <c r="I14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K14" t="s">
-        <v>18</v>
-      </c>
-      <c r="L14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C15">
         <v>2002274</v>
@@ -1442,36 +1394,33 @@
         <v>7000253824</v>
       </c>
       <c r="E15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H15">
         <v>2020</v>
       </c>
       <c r="I15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K15" t="s">
-        <v>18</v>
-      </c>
-      <c r="L15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C16">
         <v>2002275</v>
@@ -1480,36 +1429,33 @@
         <v>7000253825</v>
       </c>
       <c r="E16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H16">
         <v>2020</v>
       </c>
       <c r="I16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K16" t="s">
-        <v>18</v>
-      </c>
-      <c r="L16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C17">
         <v>2002276</v>
@@ -1518,36 +1464,33 @@
         <v>7000253826</v>
       </c>
       <c r="E17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H17">
         <v>2020</v>
       </c>
       <c r="I17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K17" t="s">
-        <v>18</v>
-      </c>
-      <c r="L17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C18">
         <v>2002277</v>
@@ -1556,36 +1499,33 @@
         <v>7000253827</v>
       </c>
       <c r="E18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H18">
         <v>2020</v>
       </c>
       <c r="I18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K18" t="s">
-        <v>18</v>
-      </c>
-      <c r="L18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C19">
         <v>2002278</v>
@@ -1594,36 +1534,33 @@
         <v>7000253828</v>
       </c>
       <c r="E19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H19">
         <v>2020</v>
       </c>
       <c r="I19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K19" t="s">
-        <v>18</v>
-      </c>
-      <c r="L19" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C20">
         <v>2002279</v>
@@ -1632,36 +1569,33 @@
         <v>7000253829</v>
       </c>
       <c r="E20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H20">
         <v>2020</v>
       </c>
       <c r="I20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K20" t="s">
-        <v>18</v>
-      </c>
-      <c r="L20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C21">
         <v>2002280</v>
@@ -1670,36 +1604,33 @@
         <v>7000253830</v>
       </c>
       <c r="E21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H21">
         <v>2020</v>
       </c>
       <c r="I21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K21" t="s">
-        <v>18</v>
-      </c>
-      <c r="L21" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C22">
         <v>2002281</v>
@@ -1708,36 +1639,33 @@
         <v>7000253831</v>
       </c>
       <c r="E22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H22">
         <v>2020</v>
       </c>
       <c r="I22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K22" t="s">
-        <v>18</v>
-      </c>
-      <c r="L22" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C23">
         <v>2002282</v>
@@ -1746,36 +1674,33 @@
         <v>7000253832</v>
       </c>
       <c r="E23" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H23">
         <v>2020</v>
       </c>
       <c r="I23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K23" t="s">
-        <v>18</v>
-      </c>
-      <c r="L23" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C24">
         <v>2002283</v>
@@ -1784,36 +1709,33 @@
         <v>7000253833</v>
       </c>
       <c r="E24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H24">
         <v>2020</v>
       </c>
       <c r="I24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K24" t="s">
-        <v>18</v>
-      </c>
-      <c r="L24" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C25">
         <v>2002284</v>
@@ -1822,36 +1744,33 @@
         <v>7000253834</v>
       </c>
       <c r="E25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H25">
         <v>2020</v>
       </c>
       <c r="I25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K25" t="s">
-        <v>18</v>
-      </c>
-      <c r="L25" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C26">
         <v>2002285</v>
@@ -1860,36 +1779,33 @@
         <v>7000253835</v>
       </c>
       <c r="E26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H26">
         <v>2020</v>
       </c>
       <c r="I26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K26" t="s">
-        <v>18</v>
-      </c>
-      <c r="L26" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C27">
         <v>2002286</v>
@@ -1898,36 +1814,33 @@
         <v>7000253836</v>
       </c>
       <c r="E27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H27">
         <v>2020</v>
       </c>
       <c r="I27" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J27" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K27" t="s">
-        <v>18</v>
-      </c>
-      <c r="L27" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C28">
         <v>2002287</v>
@@ -1936,36 +1849,33 @@
         <v>7000253837</v>
       </c>
       <c r="E28" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G28" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H28">
         <v>2020</v>
       </c>
       <c r="I28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J28" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K28" t="s">
-        <v>18</v>
-      </c>
-      <c r="L28" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C29">
         <v>2002288</v>
@@ -1974,36 +1884,33 @@
         <v>7000253838</v>
       </c>
       <c r="E29" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F29" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H29">
         <v>2020</v>
       </c>
       <c r="I29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K29" t="s">
-        <v>18</v>
-      </c>
-      <c r="L29" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C30">
         <v>2002289</v>
@@ -2012,36 +1919,33 @@
         <v>7000253839</v>
       </c>
       <c r="E30" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F30" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H30">
         <v>2020</v>
       </c>
       <c r="I30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K30" t="s">
-        <v>18</v>
-      </c>
-      <c r="L30" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C31">
         <v>2002290</v>
@@ -2050,36 +1954,33 @@
         <v>7000253840</v>
       </c>
       <c r="E31" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H31">
         <v>2020</v>
       </c>
       <c r="I31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J31" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K31" t="s">
-        <v>18</v>
-      </c>
-      <c r="L31" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C32">
         <v>2002291</v>
@@ -2088,36 +1989,33 @@
         <v>7000253841</v>
       </c>
       <c r="E32" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F32" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H32">
         <v>2020</v>
       </c>
       <c r="I32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K32" t="s">
-        <v>18</v>
-      </c>
-      <c r="L32" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C33">
         <v>2002292</v>
@@ -2126,36 +2024,33 @@
         <v>7000253842</v>
       </c>
       <c r="E33" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F33" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G33" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H33">
         <v>2020</v>
       </c>
       <c r="I33" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J33" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K33" t="s">
-        <v>18</v>
-      </c>
-      <c r="L33" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C34">
         <v>2002293</v>
@@ -2164,36 +2059,33 @@
         <v>7000253843</v>
       </c>
       <c r="E34" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F34" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H34">
         <v>2020</v>
       </c>
       <c r="I34" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J34" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K34" t="s">
-        <v>18</v>
-      </c>
-      <c r="L34" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C35">
         <v>2002294</v>
@@ -2202,36 +2094,33 @@
         <v>7000253844</v>
       </c>
       <c r="E35" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F35" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G35" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H35">
         <v>2020</v>
       </c>
       <c r="I35" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J35" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K35" t="s">
-        <v>18</v>
-      </c>
-      <c r="L35" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C36">
         <v>2002295</v>
@@ -2240,36 +2129,33 @@
         <v>7000253845</v>
       </c>
       <c r="E36" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F36" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G36" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H36">
         <v>2020</v>
       </c>
       <c r="I36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J36" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K36" t="s">
-        <v>18</v>
-      </c>
-      <c r="L36" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C37">
         <v>2002296</v>
@@ -2278,36 +2164,33 @@
         <v>7000253846</v>
       </c>
       <c r="E37" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F37" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G37" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H37">
         <v>2020</v>
       </c>
       <c r="I37" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J37" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K37" t="s">
-        <v>18</v>
-      </c>
-      <c r="L37" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C38">
         <v>2002297</v>
@@ -2316,36 +2199,33 @@
         <v>7000253847</v>
       </c>
       <c r="E38" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F38" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G38" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H38">
         <v>2020</v>
       </c>
       <c r="I38" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J38" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K38" t="s">
-        <v>18</v>
-      </c>
-      <c r="L38" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C39">
         <v>2002298</v>
@@ -2354,36 +2234,33 @@
         <v>7000253848</v>
       </c>
       <c r="E39" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F39" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G39" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H39">
         <v>2020</v>
       </c>
       <c r="I39" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J39" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K39" t="s">
-        <v>18</v>
-      </c>
-      <c r="L39" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C40">
         <v>2002299</v>
@@ -2392,36 +2269,33 @@
         <v>7000253849</v>
       </c>
       <c r="E40" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F40" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G40" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H40">
         <v>2020</v>
       </c>
       <c r="I40" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J40" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K40" t="s">
-        <v>18</v>
-      </c>
-      <c r="L40" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C41">
         <v>2002300</v>
@@ -2430,36 +2304,33 @@
         <v>7000253850</v>
       </c>
       <c r="E41" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F41" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G41" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H41">
         <v>2020</v>
       </c>
       <c r="I41" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J41" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K41" t="s">
-        <v>18</v>
-      </c>
-      <c r="L41" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C42">
         <v>2002301</v>
@@ -2468,36 +2339,33 @@
         <v>7000253851</v>
       </c>
       <c r="E42" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F42" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G42" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H42">
         <v>2020</v>
       </c>
       <c r="I42" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J42" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K42" t="s">
-        <v>18</v>
-      </c>
-      <c r="L42" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C43">
         <v>2002302</v>
@@ -2506,36 +2374,33 @@
         <v>7000253852</v>
       </c>
       <c r="E43" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F43" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G43" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H43">
         <v>2020</v>
       </c>
       <c r="I43" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J43" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K43" t="s">
-        <v>18</v>
-      </c>
-      <c r="L43" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C44">
         <v>2002303</v>
@@ -2544,36 +2409,33 @@
         <v>7000253853</v>
       </c>
       <c r="E44" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F44" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G44" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H44">
         <v>2020</v>
       </c>
       <c r="I44" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J44" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K44" t="s">
-        <v>18</v>
-      </c>
-      <c r="L44" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C45">
         <v>2002304</v>
@@ -2582,36 +2444,33 @@
         <v>7000253854</v>
       </c>
       <c r="E45" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F45" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G45" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H45">
         <v>2020</v>
       </c>
       <c r="I45" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K45" t="s">
-        <v>18</v>
-      </c>
-      <c r="L45" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C46">
         <v>2002305</v>
@@ -2620,36 +2479,33 @@
         <v>7000253855</v>
       </c>
       <c r="E46" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F46" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G46" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H46">
         <v>2020</v>
       </c>
       <c r="I46" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J46" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K46" t="s">
-        <v>18</v>
-      </c>
-      <c r="L46" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C47">
         <v>2002306</v>
@@ -2658,36 +2514,33 @@
         <v>7000253856</v>
       </c>
       <c r="E47" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F47" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G47" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H47">
         <v>2020</v>
       </c>
       <c r="I47" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J47" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K47" t="s">
-        <v>18</v>
-      </c>
-      <c r="L47" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C48">
         <v>2002307</v>
@@ -2696,36 +2549,33 @@
         <v>7000253857</v>
       </c>
       <c r="E48" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F48" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G48" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H48">
         <v>2020</v>
       </c>
       <c r="I48" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J48" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K48" t="s">
-        <v>18</v>
-      </c>
-      <c r="L48" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C49">
         <v>2002308</v>
@@ -2734,36 +2584,33 @@
         <v>7000253858</v>
       </c>
       <c r="E49" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F49" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G49" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H49">
         <v>2020</v>
       </c>
       <c r="I49" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J49" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K49" t="s">
-        <v>18</v>
-      </c>
-      <c r="L49" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C50">
         <v>2002309</v>
@@ -2772,36 +2619,33 @@
         <v>7000253859</v>
       </c>
       <c r="E50" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F50" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G50" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H50">
         <v>2020</v>
       </c>
       <c r="I50" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J50" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K50" t="s">
-        <v>18</v>
-      </c>
-      <c r="L50" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C51">
         <v>2002310</v>
@@ -2810,36 +2654,33 @@
         <v>7000253860</v>
       </c>
       <c r="E51" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F51" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G51" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H51">
         <v>2020</v>
       </c>
       <c r="I51" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J51" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K51" t="s">
-        <v>18</v>
-      </c>
-      <c r="L51" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C52">
         <v>2002311</v>
@@ -2848,36 +2689,33 @@
         <v>7000253861</v>
       </c>
       <c r="E52" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F52" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G52" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H52">
         <v>2020</v>
       </c>
       <c r="I52" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J52" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K52" t="s">
-        <v>18</v>
-      </c>
-      <c r="L52" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C53">
         <v>2002312</v>
@@ -2886,36 +2724,33 @@
         <v>7000253862</v>
       </c>
       <c r="E53" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F53" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G53" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H53">
         <v>2020</v>
       </c>
       <c r="I53" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J53" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K53" t="s">
-        <v>18</v>
-      </c>
-      <c r="L53" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C54">
         <v>2002313</v>
@@ -2924,36 +2759,33 @@
         <v>7000253863</v>
       </c>
       <c r="E54" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F54" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G54" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H54">
         <v>2020</v>
       </c>
       <c r="I54" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J54" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K54" t="s">
-        <v>18</v>
-      </c>
-      <c r="L54" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C55">
         <v>2002314</v>
@@ -2962,36 +2794,33 @@
         <v>7000253864</v>
       </c>
       <c r="E55" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F55" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G55" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H55">
         <v>2020</v>
       </c>
       <c r="I55" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J55" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K55" t="s">
-        <v>18</v>
-      </c>
-      <c r="L55" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C56">
         <v>2002315</v>
@@ -3000,36 +2829,33 @@
         <v>7000253865</v>
       </c>
       <c r="E56" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F56" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G56" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H56">
         <v>2020</v>
       </c>
       <c r="I56" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J56" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K56" t="s">
-        <v>18</v>
-      </c>
-      <c r="L56" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C57">
         <v>2002316</v>
@@ -3038,36 +2864,33 @@
         <v>7000253866</v>
       </c>
       <c r="E57" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F57" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G57" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H57">
         <v>2020</v>
       </c>
       <c r="I57" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J57" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K57" t="s">
-        <v>18</v>
-      </c>
-      <c r="L57" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C58">
         <v>2002317</v>
@@ -3076,36 +2899,33 @@
         <v>7000253867</v>
       </c>
       <c r="E58" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F58" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G58" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H58">
         <v>2020</v>
       </c>
       <c r="I58" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J58" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K58" t="s">
-        <v>18</v>
-      </c>
-      <c r="L58" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C59">
         <v>2002318</v>
@@ -3114,36 +2934,33 @@
         <v>7000253868</v>
       </c>
       <c r="E59" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F59" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G59" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H59">
         <v>2020</v>
       </c>
       <c r="I59" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J59" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K59" t="s">
-        <v>18</v>
-      </c>
-      <c r="L59" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C60">
         <v>2002319</v>
@@ -3152,36 +2969,33 @@
         <v>7000253869</v>
       </c>
       <c r="E60" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F60" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G60" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H60">
         <v>2020</v>
       </c>
       <c r="I60" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J60" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K60" t="s">
-        <v>18</v>
-      </c>
-      <c r="L60" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C61">
         <v>2002320</v>
@@ -3190,28 +3004,25 @@
         <v>7000253870</v>
       </c>
       <c r="E61" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F61" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G61" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H61">
         <v>2020</v>
       </c>
       <c r="I61" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J61" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K61" t="s">
-        <v>18</v>
-      </c>
-      <c r="L61" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>